<commit_message>
added diagram and changed report
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rauzh\source\repos\LW1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Часть 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Часть 2" sheetId="2" r:id="rId2"/>
+    <sheet name="первая задача" sheetId="1" r:id="rId1"/>
+    <sheet name="вторая задача" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Возрастание</t>
   </si>
@@ -50,11 +45,14 @@
   <si>
     <t>Дробные Числа</t>
   </si>
+  <si>
+    <t>Количество элементов</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,7 +70,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -174,11 +172,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -195,6 +266,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -214,7 +292,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -262,26 +340,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -309,7 +367,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$A$3:$A$202</c:f>
+              <c:f>'первая задача'!$A$3:$A$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -917,7 +975,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-73F8-4BB4-B5A6-58CDBD484618}"/>
             </c:ext>
@@ -943,7 +1001,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$B$3:$B$202</c:f>
+              <c:f>'первая задача'!$B$3:$B$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -1551,7 +1609,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-73F8-4BB4-B5A6-58CDBD484618}"/>
             </c:ext>
@@ -1577,7 +1635,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$C$3:$C$202</c:f>
+              <c:f>'первая задача'!$C$3:$C$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -2185,7 +2243,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-73F8-4BB4-B5A6-58CDBD484618}"/>
             </c:ext>
@@ -2199,12 +2257,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2095110720"/>
-        <c:axId val="2095111552"/>
+        <c:axId val="173070848"/>
+        <c:axId val="209276864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2095110720"/>
+        <c:axId val="173070848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,10 +2302,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095111552"/>
+        <c:crossAx val="209276864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2254,7 +2313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095111552"/>
+        <c:axId val="209276864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,10 +2361,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095110720"/>
+        <c:crossAx val="173070848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2345,7 +2404,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2375,7 +2434,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2387,7 +2446,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2440,26 +2499,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2487,7 +2526,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$D$3:$D$202</c:f>
+              <c:f>'первая задача'!$D$3:$D$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -3095,7 +3134,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-019E-4600-85E4-CFF93DF24B32}"/>
             </c:ext>
@@ -3121,7 +3160,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$E$3:$E$202</c:f>
+              <c:f>'первая задача'!$E$3:$E$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -3729,7 +3768,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-019E-4600-85E4-CFF93DF24B32}"/>
             </c:ext>
@@ -3755,7 +3794,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$F$3:$F$202</c:f>
+              <c:f>'первая задача'!$F$3:$F$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -4363,7 +4402,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-019E-4600-85E4-CFF93DF24B32}"/>
             </c:ext>
@@ -4377,12 +4416,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125504576"/>
-        <c:axId val="2125511648"/>
+        <c:axId val="184329728"/>
+        <c:axId val="209278592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125504576"/>
+        <c:axId val="184329728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4421,10 +4461,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125511648"/>
+        <c:crossAx val="209278592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4432,7 +4472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125511648"/>
+        <c:axId val="209278592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4480,10 +4520,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125504576"/>
+        <c:crossAx val="184329728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4523,7 +4563,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4553,7 +4593,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4565,7 +4605,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -4613,26 +4653,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4660,7 +4680,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$G$3:$G$202</c:f>
+              <c:f>'первая задача'!$G$3:$G$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -5268,7 +5288,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D247-4837-8807-C255DBD0E77C}"/>
             </c:ext>
@@ -5294,7 +5314,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$H$3:$H$202</c:f>
+              <c:f>'первая задача'!$H$3:$H$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -5902,7 +5922,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D247-4837-8807-C255DBD0E77C}"/>
             </c:ext>
@@ -5928,7 +5948,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$I$3:$I$202</c:f>
+              <c:f>'первая задача'!$I$3:$I$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -6536,7 +6556,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D247-4837-8807-C255DBD0E77C}"/>
             </c:ext>
@@ -6550,12 +6570,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091881792"/>
-        <c:axId val="2091874304"/>
+        <c:axId val="184330240"/>
+        <c:axId val="209280320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091881792"/>
+        <c:axId val="184330240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6594,10 +6615,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091874304"/>
+        <c:crossAx val="209280320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6605,7 +6626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091874304"/>
+        <c:axId val="209280320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6653,10 +6674,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091881792"/>
+        <c:crossAx val="184330240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6696,7 +6717,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6726,7 +6747,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6738,7 +6759,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -6786,26 +6807,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -6833,7 +6834,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$J$3:$J$202</c:f>
+              <c:f>'первая задача'!$J$3:$J$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -7441,7 +7442,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-83B6-48AD-9DB7-C25C840BB1A4}"/>
             </c:ext>
@@ -7467,7 +7468,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$K$3:$K$202</c:f>
+              <c:f>'первая задача'!$K$3:$K$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -8075,7 +8076,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-83B6-48AD-9DB7-C25C840BB1A4}"/>
             </c:ext>
@@ -8101,7 +8102,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Часть 1'!$L$3:$L$202</c:f>
+              <c:f>'первая задача'!$L$3:$L$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -8709,7 +8710,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-83B6-48AD-9DB7-C25C840BB1A4}"/>
             </c:ext>
@@ -8723,12 +8724,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091877632"/>
-        <c:axId val="2091882208"/>
+        <c:axId val="184330752"/>
+        <c:axId val="185074816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091877632"/>
+        <c:axId val="184330752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8767,10 +8769,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091882208"/>
+        <c:crossAx val="185074816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8778,7 +8780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091882208"/>
+        <c:axId val="185074816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8826,10 +8828,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091877632"/>
+        <c:crossAx val="184330752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8869,7 +8871,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8899,9 +8901,666 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'вторая задача'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Возрастание</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'вторая задача'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'вторая задача'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3877</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7082</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8118</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9969</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10607</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11893</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'вторая задача'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Убывание</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'вторая задача'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'вторая задача'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3616</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5865</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8740</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10924</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11817</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'вторая задача'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Случайная</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'вторая задача'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'вторая задача'!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20790</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42542</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62616</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86555</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101866</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128830</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>147303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>166039</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>191574</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>206258</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'вторая задача'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Синусоидальная</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'вторая задача'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'вторая задача'!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7646</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31904</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35080</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'вторая задача'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Пилообразная</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'вторая задача'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'вторая задача'!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13818</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39852</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80213</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106449</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>118704</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>134314</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'вторая задача'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ступенчатая</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'вторая задача'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'вторая задача'!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63488</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86882</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>124977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>167247</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189237</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>211274</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="160757760"/>
+        <c:axId val="186517760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="160757760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="186517760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="186517760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="160757760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="0"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -11259,6 +11918,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>128586</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -11514,7 +12208,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11524,20 +12218,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V51" sqref="V51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -11555,7 +12249,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -11593,7 +12287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -11631,7 +12325,7 @@
         <v>20.668661</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -11669,7 +12363,7 @@
         <v>-21.401105000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -11707,7 +12401,7 @@
         <v>6.5538499999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -11745,7 +12439,7 @@
         <v>-9.1784420000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>20</v>
       </c>
@@ -11783,7 +12477,7 @@
         <v>-36.526077999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>25</v>
       </c>
@@ -11821,7 +12515,7 @@
         <v>29.653310000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>30</v>
       </c>
@@ -11859,7 +12553,7 @@
         <v>47.213659999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>35</v>
       </c>
@@ -11897,7 +12591,7 @@
         <v>-9.269997</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>40</v>
       </c>
@@ -11935,7 +12629,7 @@
         <v>-11.87933</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44</v>
       </c>
@@ -11973,7 +12667,7 @@
         <v>12.453078</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>49</v>
       </c>
@@ -12011,7 +12705,7 @@
         <v>38.924833</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>54</v>
       </c>
@@ -12049,7 +12743,7 @@
         <v>-35.805841000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>60</v>
       </c>
@@ -12087,7 +12781,7 @@
         <v>15.092929</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>65</v>
       </c>
@@ -12125,7 +12819,7 @@
         <v>9.9414040000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>70</v>
       </c>
@@ -12163,7 +12857,7 @@
         <v>49.728385000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>75</v>
       </c>
@@ -12201,7 +12895,7 @@
         <v>6.556902</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>80</v>
       </c>
@@ -12239,7 +12933,7 @@
         <v>9.9810789999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>85</v>
       </c>
@@ -12277,7 +12971,7 @@
         <v>20.513016</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>90</v>
       </c>
@@ -12315,7 +13009,7 @@
         <v>48.931851999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>95</v>
       </c>
@@ -12353,7 +13047,7 @@
         <v>-33.608508999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>100</v>
       </c>
@@ -12391,7 +13085,7 @@
         <v>7.5579090000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>105</v>
       </c>
@@ -12429,7 +13123,7 @@
         <v>48.278756000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>110</v>
       </c>
@@ -12467,7 +13161,7 @@
         <v>48.861660000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>115</v>
       </c>
@@ -12505,7 +13199,7 @@
         <v>-17.259743</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>120</v>
       </c>
@@ -12543,7 +13237,7 @@
         <v>12.639241</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>125</v>
       </c>
@@ -12581,7 +13275,7 @@
         <v>-36.968595999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>130</v>
       </c>
@@ -12619,7 +13313,7 @@
         <v>37.450789</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>135</v>
       </c>
@@ -12657,7 +13351,7 @@
         <v>49.856563000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>140</v>
       </c>
@@ -12695,7 +13389,7 @@
         <v>18.294321</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>145</v>
       </c>
@@ -12733,7 +13427,7 @@
         <v>8.0736720000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>150</v>
       </c>
@@ -12771,7 +13465,7 @@
         <v>-32.732627000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>155</v>
       </c>
@@ -12809,7 +13503,7 @@
         <v>12.630084999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>160</v>
       </c>
@@ -12847,7 +13541,7 @@
         <v>32.085635000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>165</v>
       </c>
@@ -12885,7 +13579,7 @@
         <v>-15.981017</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>170</v>
       </c>
@@ -12923,7 +13617,7 @@
         <v>16.606646999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>175</v>
       </c>
@@ -12961,7 +13655,7 @@
         <v>45.803705000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>180</v>
       </c>
@@ -12999,7 +13693,7 @@
         <v>-49.081392999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>185</v>
       </c>
@@ -13037,7 +13731,7 @@
         <v>-13.313700000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>190</v>
       </c>
@@ -13075,7 +13769,7 @@
         <v>-11.726737</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>195</v>
       </c>
@@ -13113,7 +13807,7 @@
         <v>20.094912999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>200</v>
       </c>
@@ -13151,7 +13845,7 @@
         <v>175.20523700000001</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>205</v>
       </c>
@@ -13189,7 +13883,7 @@
         <v>227.24845099999999</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>210</v>
       </c>
@@ -13227,7 +13921,7 @@
         <v>161.70995199999999</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>215</v>
       </c>
@@ -13265,7 +13959,7 @@
         <v>208.360546</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>220</v>
       </c>
@@ -13303,7 +13997,7 @@
         <v>202.81533200000001</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>225</v>
       </c>
@@ -13341,7 +14035,7 @@
         <v>212.69112200000001</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>229</v>
       </c>
@@ -13379,7 +14073,7 @@
         <v>164.05072200000001</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>234</v>
       </c>
@@ -13417,7 +14111,7 @@
         <v>234.93301199999999</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>239</v>
       </c>
@@ -13455,7 +14149,7 @@
         <v>193.63536500000001</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>244</v>
       </c>
@@ -13493,7 +14187,7 @@
         <v>214.77858800000001</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>249</v>
       </c>
@@ -13531,7 +14225,7 @@
         <v>175.73320699999999</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>254</v>
       </c>
@@ -13569,7 +14263,7 @@
         <v>221.21494200000001</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>259</v>
       </c>
@@ -13607,7 +14301,7 @@
         <v>245.19638699999999</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>264</v>
       </c>
@@ -13645,7 +14339,7 @@
         <v>205.62913900000001</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>269</v>
       </c>
@@ -13683,7 +14377,7 @@
         <v>236.34601900000001</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>274</v>
       </c>
@@ -13721,7 +14415,7 @@
         <v>230.74587199999999</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>279</v>
       </c>
@@ -13759,7 +14453,7 @@
         <v>170.072024</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>284</v>
       </c>
@@ -13797,7 +14491,7 @@
         <v>187.96807799999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>289</v>
       </c>
@@ -13835,7 +14529,7 @@
         <v>166.238899</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>294</v>
       </c>
@@ -13873,7 +14567,7 @@
         <v>166.73940200000001</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>299</v>
       </c>
@@ -13911,7 +14605,7 @@
         <v>215.694143</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>304</v>
       </c>
@@ -13949,7 +14643,7 @@
         <v>198.29859300000001</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>309</v>
       </c>
@@ -13987,7 +14681,7 @@
         <v>169.656972</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>314</v>
       </c>
@@ -14025,7 +14719,7 @@
         <v>225.34409600000001</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>319</v>
       </c>
@@ -14063,7 +14757,7 @@
         <v>217.11020199999999</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>324</v>
       </c>
@@ -14101,7 +14795,7 @@
         <v>210.991241</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>329</v>
       </c>
@@ -14139,7 +14833,7 @@
         <v>234.85366400000001</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>334</v>
       </c>
@@ -14177,7 +14871,7 @@
         <v>157.64488700000001</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>339</v>
       </c>
@@ -14215,7 +14909,7 @@
         <v>223.44584499999999</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>344</v>
       </c>
@@ -14253,7 +14947,7 @@
         <v>221.50792000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>349</v>
       </c>
@@ -14291,7 +14985,7 @@
         <v>196.967986</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>354</v>
       </c>
@@ -14329,7 +15023,7 @@
         <v>243.627735</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>359</v>
       </c>
@@ -14367,7 +15061,7 @@
         <v>188.56623999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>364</v>
       </c>
@@ -14405,7 +15099,7 @@
         <v>236.84652199999999</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>369</v>
       </c>
@@ -14443,7 +15137,7 @@
         <v>179.20011</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>374</v>
       </c>
@@ -14481,7 +15175,7 @@
         <v>231.124302</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>379</v>
       </c>
@@ -14519,7 +15213,7 @@
         <v>166.65700200000001</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>384</v>
       </c>
@@ -14557,7 +15251,7 @@
         <v>151.33060699999999</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>389</v>
       </c>
@@ -14595,7 +15289,7 @@
         <v>177.92443599999999</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>394</v>
       </c>
@@ -14633,7 +15327,7 @@
         <v>242.98074299999999</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>399</v>
       </c>
@@ -14671,7 +15365,7 @@
         <v>403.30668100000003</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>404</v>
       </c>
@@ -14709,7 +15403,7 @@
         <v>435.88518900000003</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>409</v>
       </c>
@@ -14747,7 +15441,7 @@
         <v>407.37785000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>414</v>
       </c>
@@ -14785,7 +15479,7 @@
         <v>405.47044299999999</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>419</v>
       </c>
@@ -14823,7 +15517,7 @@
         <v>362.69264800000002</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>424</v>
       </c>
@@ -14861,7 +15555,7 @@
         <v>418.895535</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>429</v>
       </c>
@@ -14899,7 +15593,7 @@
         <v>369.55015700000001</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>434</v>
       </c>
@@ -14937,7 +15631,7 @@
         <v>401.15207400000003</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>439</v>
       </c>
@@ -14975,7 +15669,7 @@
         <v>381.57750199999998</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>444</v>
       </c>
@@ -15013,7 +15707,7 @@
         <v>386.820582</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>449</v>
       </c>
@@ -15051,7 +15745,7 @@
         <v>364.88692900000001</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>454</v>
       </c>
@@ -15089,7 +15783,7 @@
         <v>399.24466699999999</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>459</v>
       </c>
@@ -15127,7 +15821,7 @@
         <v>390.63844699999999</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>464</v>
       </c>
@@ -15165,7 +15859,7 @@
         <v>382.63038999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>469</v>
       </c>
@@ -15203,7 +15897,7 @@
         <v>409.45005600000002</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>474</v>
       </c>
@@ -15241,7 +15935,7 @@
         <v>366.66921000000002</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>479</v>
       </c>
@@ -15279,7 +15973,7 @@
         <v>393.83678700000002</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>484</v>
       </c>
@@ -15317,7 +16011,7 @@
         <v>430.24231700000001</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>489</v>
       </c>
@@ -15355,7 +16049,7 @@
         <v>374.109622</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>494</v>
       </c>
@@ -15393,7 +16087,7 @@
         <v>412.90475199999997</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>499</v>
       </c>
@@ -15431,7 +16125,7 @@
         <v>446.40186799999998</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>504</v>
       </c>
@@ -15469,7 +16163,7 @@
         <v>363.03445499999998</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>509</v>
       </c>
@@ -15507,7 +16201,7 @@
         <v>411.50395200000003</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>514</v>
       </c>
@@ -15545,7 +16239,7 @@
         <v>371.70781599999998</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>519</v>
       </c>
@@ -15583,7 +16277,7 @@
         <v>422.07556399999999</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>524</v>
       </c>
@@ -15621,7 +16315,7 @@
         <v>384.62630100000001</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>529</v>
       </c>
@@ -15659,7 +16353,7 @@
         <v>386.23767800000002</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>534</v>
       </c>
@@ -15697,7 +16391,7 @@
         <v>372.93771199999998</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>539</v>
       </c>
@@ -15735,7 +16429,7 @@
         <v>410.26184899999998</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>544</v>
       </c>
@@ -15773,7 +16467,7 @@
         <v>439.953307</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>549</v>
       </c>
@@ -15811,7 +16505,7 @@
         <v>374.08520800000002</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>554</v>
       </c>
@@ -15849,7 +16543,7 @@
         <v>407.48466400000001</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>559</v>
       </c>
@@ -15887,7 +16581,7 @@
         <v>433.64513099999999</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>564</v>
       </c>
@@ -15925,7 +16619,7 @@
         <v>424.871059</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>569</v>
       </c>
@@ -15963,7 +16657,7 @@
         <v>445.73961600000001</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>574</v>
       </c>
@@ -16001,7 +16695,7 @@
         <v>438.51893699999999</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>579</v>
       </c>
@@ -16039,7 +16733,7 @@
         <v>426.97683599999999</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>584</v>
       </c>
@@ -16077,7 +16771,7 @@
         <v>412.32795199999998</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>589</v>
       </c>
@@ -16115,7 +16809,7 @@
         <v>400.74922900000001</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>594</v>
       </c>
@@ -16153,7 +16847,7 @@
         <v>362.15552200000002</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>599</v>
       </c>
@@ -16191,7 +16885,7 @@
         <v>567.590869</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>604</v>
       </c>
@@ -16229,7 +16923,7 @@
         <v>623.28409699999997</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>609</v>
       </c>
@@ -16267,7 +16961,7 @@
         <v>567.30704700000001</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>614</v>
       </c>
@@ -16305,7 +16999,7 @@
         <v>570.636616</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>619</v>
       </c>
@@ -16343,7 +17037,7 @@
         <v>598.33826699999997</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>624</v>
       </c>
@@ -16381,7 +17075,7 @@
         <v>620.47028999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>629</v>
       </c>
@@ -16419,7 +17113,7 @@
         <v>633.44676000000004</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>634</v>
       </c>
@@ -16457,7 +17151,7 @@
         <v>621.20578599999999</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>639</v>
       </c>
@@ -16495,7 +17189,7 @@
         <v>633.483383</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>644</v>
       </c>
@@ -16533,7 +17227,7 @@
         <v>553.12204399999996</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>649</v>
       </c>
@@ -16571,7 +17265,7 @@
         <v>625.32273299999997</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>654</v>
       </c>
@@ -16609,7 +17303,7 @@
         <v>563.74248499999999</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>659</v>
       </c>
@@ -16647,7 +17341,7 @@
         <v>588.27021100000002</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>664</v>
       </c>
@@ -16685,7 +17379,7 @@
         <v>630.83437600000002</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>669</v>
       </c>
@@ -16723,7 +17417,7 @@
         <v>598.21314099999995</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>674</v>
       </c>
@@ -16761,7 +17455,7 @@
         <v>630.33692399999995</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>679</v>
       </c>
@@ -16799,7 +17493,7 @@
         <v>622.73171200000002</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>684</v>
       </c>
@@ -16837,7 +17531,7 @@
         <v>554.59913900000004</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>689</v>
       </c>
@@ -16875,7 +17569,7 @@
         <v>555.79241300000001</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>694</v>
       </c>
@@ -16913,7 +17607,7 @@
         <v>639.88311399999998</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>699</v>
       </c>
@@ -16951,7 +17645,7 @@
         <v>640.38666999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>704</v>
       </c>
@@ -16989,7 +17683,7 @@
         <v>583.265175</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>709</v>
       </c>
@@ -17027,7 +17721,7 @@
         <v>563.39457400000003</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>714</v>
       </c>
@@ -17065,7 +17759,7 @@
         <v>620.85482300000001</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>719</v>
       </c>
@@ -17103,7 +17797,7 @@
         <v>632.43049399999995</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>724</v>
       </c>
@@ -17141,7 +17835,7 @@
         <v>563.39457400000003</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>729</v>
       </c>
@@ -17179,7 +17873,7 @@
         <v>570.81667500000003</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>734</v>
       </c>
@@ -17217,7 +17911,7 @@
         <v>605.34836900000005</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>739</v>
       </c>
@@ -17255,7 +17949,7 @@
         <v>608.08282699999995</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>744</v>
       </c>
@@ -17293,7 +17987,7 @@
         <v>600.78585199999998</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>749</v>
       </c>
@@ -17331,7 +18025,7 @@
         <v>610.33509300000003</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>754</v>
       </c>
@@ -17369,7 +18063,7 @@
         <v>597.566149</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>759</v>
       </c>
@@ -17407,7 +18101,7 @@
         <v>601.67088799999999</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>764</v>
       </c>
@@ -17445,7 +18139,7 @@
         <v>601.67699200000004</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>769</v>
       </c>
@@ -17483,7 +18177,7 @@
         <v>585.52964899999995</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>774</v>
       </c>
@@ -17521,7 +18215,7 @@
         <v>569.80956500000002</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>779</v>
       </c>
@@ -17559,7 +18253,7 @@
         <v>597.11142299999995</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>784</v>
       </c>
@@ -17597,7 +18291,7 @@
         <v>561.841182</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>789</v>
       </c>
@@ -17635,7 +18329,7 @@
         <v>616.57002499999999</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>794</v>
       </c>
@@ -17673,7 +18367,7 @@
         <v>589.16745500000002</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>799</v>
       </c>
@@ -17711,7 +18405,7 @@
         <v>760.38239699999997</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>804</v>
       </c>
@@ -17749,7 +18443,7 @@
         <v>831.61870199999998</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>809</v>
       </c>
@@ -17787,7 +18481,7 @@
         <v>757.55638299999998</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>814</v>
       </c>
@@ -17825,7 +18519,7 @@
         <v>827.96258399999999</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>819</v>
       </c>
@@ -17863,7 +18557,7 @@
         <v>820.65950499999997</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>824</v>
       </c>
@@ -17901,7 +18595,7 @@
         <v>835.07950100000005</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>829</v>
       </c>
@@ -17939,7 +18633,7 @@
         <v>751.55339200000003</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>834</v>
       </c>
@@ -17977,7 +18671,7 @@
         <v>761.13620400000002</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>839</v>
       </c>
@@ -18015,7 +18709,7 @@
         <v>790.65675799999997</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>844</v>
       </c>
@@ -18053,7 +18747,7 @@
         <v>771.40263100000004</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>849</v>
       </c>
@@ -18091,7 +18785,7 @@
         <v>838.97366299999999</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>854</v>
       </c>
@@ -18129,7 +18823,7 @@
         <v>803.66069500000003</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>859</v>
       </c>
@@ -18167,7 +18861,7 @@
         <v>766.91946199999995</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>864</v>
       </c>
@@ -18205,7 +18899,7 @@
         <v>776.60603700000001</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>869</v>
       </c>
@@ -18243,7 +18937,7 @@
         <v>784.84908600000006</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>874</v>
       </c>
@@ -18281,7 +18975,7 @@
         <v>791.11758799999996</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>879</v>
       </c>
@@ -18319,7 +19013,7 @@
         <v>800.56611799999996</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>884</v>
       </c>
@@ -18357,7 +19051,7 @@
         <v>773.75560800000005</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>889</v>
       </c>
@@ -18395,7 +19089,7 @@
         <v>840.75289199999997</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>894</v>
       </c>
@@ -18433,7 +19127,7 @@
         <v>756.56453099999999</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>899</v>
       </c>
@@ -18471,7 +19165,7 @@
         <v>779.18485099999998</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>904</v>
       </c>
@@ -18509,7 +19203,7 @@
         <v>789.76867000000004</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>909</v>
       </c>
@@ -18547,7 +19241,7 @@
         <v>806.82851600000004</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>914</v>
       </c>
@@ -18585,7 +19279,7 @@
         <v>806.81936099999996</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>919</v>
       </c>
@@ -18623,7 +19317,7 @@
         <v>810.50294499999995</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>924</v>
       </c>
@@ -18661,7 +19355,7 @@
         <v>766.94997999999998</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>929</v>
       </c>
@@ -18699,7 +19393,7 @@
         <v>809.71861899999999</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>934</v>
       </c>
@@ -18737,7 +19431,7 @@
         <v>751.27872600000001</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>939</v>
       </c>
@@ -18775,7 +19469,7 @@
         <v>848.409986</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>944</v>
       </c>
@@ -18813,7 +19507,7 @@
         <v>847.39371900000003</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>950</v>
       </c>
@@ -18851,7 +19545,7 @@
         <v>761.87780399999997</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>955</v>
       </c>
@@ -18889,7 +19583,7 @@
         <v>786.40247799999997</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>960</v>
       </c>
@@ -18927,7 +19621,7 @@
         <v>752.00811799999997</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>965</v>
       </c>
@@ -18965,7 +19659,7 @@
         <v>758.32239800000002</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>970</v>
       </c>
@@ -19003,7 +19697,7 @@
         <v>818.00439500000005</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>975</v>
       </c>
@@ -19041,7 +19735,7 @@
         <v>788.98739599999999</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>980</v>
       </c>
@@ -19079,7 +19773,7 @@
         <v>818.297372</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>985</v>
       </c>
@@ -19117,7 +19811,7 @@
         <v>776.57551799999999</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>990</v>
       </c>
@@ -19155,7 +19849,7 @@
         <v>794.11450500000001</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>995</v>
       </c>
@@ -19206,12 +19900,279 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>500000</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1150</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1160</v>
+      </c>
+      <c r="D2" s="4">
+        <v>20790</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3799</v>
+      </c>
+      <c r="F2" s="4">
+        <v>13818</v>
+      </c>
+      <c r="G2" s="4">
+        <v>20964</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>1000000</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2287</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2431</v>
+      </c>
+      <c r="D3" s="9">
+        <v>42542</v>
+      </c>
+      <c r="E3" s="9">
+        <v>7646</v>
+      </c>
+      <c r="F3" s="9">
+        <v>26009</v>
+      </c>
+      <c r="G3" s="9">
+        <v>41599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>1500000</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3877</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3616</v>
+      </c>
+      <c r="D4" s="9">
+        <v>62616</v>
+      </c>
+      <c r="E4" s="9">
+        <v>12197</v>
+      </c>
+      <c r="F4" s="9">
+        <v>39852</v>
+      </c>
+      <c r="G4" s="9">
+        <v>63488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="B5" s="10">
+        <v>4664</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5449</v>
+      </c>
+      <c r="D5" s="9">
+        <v>86555</v>
+      </c>
+      <c r="E5" s="9">
+        <v>15446</v>
+      </c>
+      <c r="F5" s="9">
+        <v>52938</v>
+      </c>
+      <c r="G5" s="9">
+        <v>86882</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>2500000</v>
+      </c>
+      <c r="B6" s="10">
+        <v>5914</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5865</v>
+      </c>
+      <c r="D6" s="9">
+        <v>101866</v>
+      </c>
+      <c r="E6" s="9">
+        <v>19930</v>
+      </c>
+      <c r="F6" s="9">
+        <v>71615</v>
+      </c>
+      <c r="G6" s="9">
+        <v>105312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>3000000</v>
+      </c>
+      <c r="B7" s="10">
+        <v>7082</v>
+      </c>
+      <c r="C7" s="9">
+        <v>7059</v>
+      </c>
+      <c r="D7" s="9">
+        <v>128830</v>
+      </c>
+      <c r="E7" s="9">
+        <v>23222</v>
+      </c>
+      <c r="F7" s="9">
+        <v>80213</v>
+      </c>
+      <c r="G7" s="9">
+        <v>124977</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>3500000</v>
+      </c>
+      <c r="B8" s="10">
+        <v>8118</v>
+      </c>
+      <c r="C8" s="9">
+        <v>8740</v>
+      </c>
+      <c r="D8" s="9">
+        <v>147303</v>
+      </c>
+      <c r="E8" s="9">
+        <v>26994</v>
+      </c>
+      <c r="F8" s="9">
+        <v>92225</v>
+      </c>
+      <c r="G8" s="9">
+        <v>146000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>4000000</v>
+      </c>
+      <c r="B9" s="10">
+        <v>9969</v>
+      </c>
+      <c r="C9" s="9">
+        <v>9750</v>
+      </c>
+      <c r="D9" s="9">
+        <v>166039</v>
+      </c>
+      <c r="E9" s="9">
+        <v>31904</v>
+      </c>
+      <c r="F9" s="9">
+        <v>106449</v>
+      </c>
+      <c r="G9" s="9">
+        <v>167247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>4500000</v>
+      </c>
+      <c r="B10" s="10">
+        <v>10607</v>
+      </c>
+      <c r="C10" s="9">
+        <v>10924</v>
+      </c>
+      <c r="D10" s="9">
+        <v>191574</v>
+      </c>
+      <c r="E10" s="9">
+        <v>35080</v>
+      </c>
+      <c r="F10" s="9">
+        <v>118704</v>
+      </c>
+      <c r="G10" s="9">
+        <v>189237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>5000000</v>
+      </c>
+      <c r="B11" s="10">
+        <v>11893</v>
+      </c>
+      <c r="C11" s="9">
+        <v>11817</v>
+      </c>
+      <c r="D11" s="9">
+        <v>206258</v>
+      </c>
+      <c r="E11" s="9">
+        <v>38313</v>
+      </c>
+      <c r="F11" s="9">
+        <v>134314</v>
+      </c>
+      <c r="G11" s="9">
+        <v>211274</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>